<commit_message>
final usina dia 02 dez 14
</commit_message>
<xml_diff>
--- a/xls/calculo_disponibilidade.xlsx
+++ b/xls/calculo_disponibilidade.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="familias">Plan1!$T$38:$U$50</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="66">
   <si>
     <t>indice_ld</t>
   </si>
@@ -85,6 +88,135 @@
   </si>
   <si>
     <t>histograma da Aciaria 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 01 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 02 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 03 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 04 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 05 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 06 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 07 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 08 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 09 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 11 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 12 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 13 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 14 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 15 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 16 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 17 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 18 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 19 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 20 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 21 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 22 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 23 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 24 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 25 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 26 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 27 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 28 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 29 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 30 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dia 31 </t>
+  </si>
+  <si>
+    <t>campanha1</t>
+  </si>
+  <si>
+    <t>campanha2</t>
+  </si>
+  <si>
+    <t>ld1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ld2         </t>
+  </si>
+  <si>
+    <t>parada1</t>
+  </si>
+  <si>
+    <t>parada2</t>
+  </si>
+  <si>
+    <t>paradaRH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inspecao1   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inspecao2   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">paradaMLC1  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">paradaMLC2  </t>
+  </si>
+  <si>
+    <t>Acerto</t>
   </si>
 </sst>
 </file>
@@ -436,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:U50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="Q44" sqref="Q44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2:T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -447,9 +579,10 @@
     <col min="6" max="6" width="1.6640625" customWidth="1"/>
     <col min="8" max="8" width="1.6640625" customWidth="1"/>
     <col min="14" max="14" width="1.6640625" customWidth="1"/>
+    <col min="20" max="20" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,8 +616,11 @@
       <c r="O1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="T1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2">
         <v>1</v>
       </c>
@@ -519,8 +655,22 @@
       <c r="O2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="Q2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2" t="str">
+        <f>VLOOKUP(R2,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T2" t="b">
+        <f>S2=G2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3">
         <v>1</v>
       </c>
@@ -555,8 +705,22 @@
       <c r="O3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="Q3" t="s">
+        <v>24</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3" t="str">
+        <f>VLOOKUP(R3,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T3" t="b">
+        <f t="shared" ref="T3:T32" si="1">S3=G3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
       <c r="A4">
         <v>1</v>
       </c>
@@ -591,8 +755,22 @@
       <c r="O4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="Q4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4">
+        <v>8</v>
+      </c>
+      <c r="S4" t="str">
+        <f>VLOOKUP(R4,familias,2,FALSE)</f>
+        <v>paradaRH</v>
+      </c>
+      <c r="T4" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5">
         <v>1</v>
       </c>
@@ -609,7 +787,7 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
@@ -627,8 +805,22 @@
       <c r="O5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="Q5" t="s">
+        <v>26</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5" t="str">
+        <f>VLOOKUP(R5,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T5" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6">
         <v>1</v>
       </c>
@@ -645,7 +837,7 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
@@ -663,8 +855,22 @@
       <c r="O6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="Q6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6" t="str">
+        <f>VLOOKUP(R6,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T6" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
       <c r="A7">
         <v>1</v>
       </c>
@@ -681,7 +887,7 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
@@ -699,8 +905,22 @@
       <c r="O7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="Q7" t="s">
+        <v>28</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7" t="str">
+        <f>VLOOKUP(R7,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T7" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
       <c r="A8">
         <v>1</v>
       </c>
@@ -717,7 +937,7 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
@@ -735,8 +955,22 @@
       <c r="O8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="Q8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8" t="str">
+        <f>VLOOKUP(R8,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T8" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
       <c r="A9">
         <v>1</v>
       </c>
@@ -771,8 +1005,22 @@
       <c r="O9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="Q9" t="s">
+        <v>30</v>
+      </c>
+      <c r="R9">
+        <v>8</v>
+      </c>
+      <c r="S9" t="str">
+        <f>VLOOKUP(R9,familias,2,FALSE)</f>
+        <v>paradaRH</v>
+      </c>
+      <c r="T9" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
       <c r="A10">
         <v>1</v>
       </c>
@@ -807,8 +1055,22 @@
       <c r="O10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="Q10" t="s">
+        <v>31</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10" t="str">
+        <f>VLOOKUP(R10,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T10" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
       <c r="A11">
         <v>1</v>
       </c>
@@ -843,8 +1105,22 @@
       <c r="O11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="Q11" t="s">
+        <v>32</v>
+      </c>
+      <c r="R11">
+        <v>12</v>
+      </c>
+      <c r="S11" t="str">
+        <f>VLOOKUP(R11,familias,2,FALSE)</f>
+        <v xml:space="preserve">paradaMLC2  </v>
+      </c>
+      <c r="T11" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
       <c r="A12">
         <v>1</v>
       </c>
@@ -879,8 +1155,22 @@
       <c r="O12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="Q12" t="s">
+        <v>33</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12" t="str">
+        <f>VLOOKUP(R12,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T12" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
       <c r="A13">
         <v>1</v>
       </c>
@@ -915,8 +1205,22 @@
       <c r="O13" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="Q13" t="s">
+        <v>34</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13" t="str">
+        <f>VLOOKUP(R13,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T13" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
       <c r="A14">
         <v>0.33333000000000002</v>
       </c>
@@ -951,8 +1255,22 @@
       <c r="O14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="Q14" t="s">
+        <v>35</v>
+      </c>
+      <c r="R14">
+        <v>10</v>
+      </c>
+      <c r="S14" t="str">
+        <f>VLOOKUP(R14,familias,2,FALSE)</f>
+        <v xml:space="preserve">inspecao2   </v>
+      </c>
+      <c r="T14" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
       <c r="A15">
         <v>1</v>
       </c>
@@ -987,8 +1305,22 @@
       <c r="O15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="Q15" t="s">
+        <v>36</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15" t="str">
+        <f>VLOOKUP(R15,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T15" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1023,8 +1355,22 @@
       <c r="O16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="Q16" t="s">
+        <v>37</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16" t="str">
+        <f>VLOOKUP(R16,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T16" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1059,8 +1405,22 @@
       <c r="O17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="Q17" t="s">
+        <v>38</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17" t="str">
+        <f>VLOOKUP(R17,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T17" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1095,8 +1455,22 @@
       <c r="O18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="Q18" t="s">
+        <v>39</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18" t="str">
+        <f>VLOOKUP(R18,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T18" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1113,7 +1487,7 @@
         <v>0.5</v>
       </c>
       <c r="G19" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="I19">
         <f t="shared" si="0"/>
@@ -1131,8 +1505,22 @@
       <c r="O19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="Q19" t="s">
+        <v>40</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19" t="str">
+        <f>VLOOKUP(R19,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T19" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1167,8 +1555,22 @@
       <c r="O20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="Q20" t="s">
+        <v>41</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20" t="str">
+        <f>VLOOKUP(R20,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T20" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1203,8 +1605,22 @@
       <c r="O21" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="Q21" t="s">
+        <v>42</v>
+      </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="S21" t="str">
+        <f>VLOOKUP(R21,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T21" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1239,8 +1655,22 @@
       <c r="O22" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="Q22" t="s">
+        <v>43</v>
+      </c>
+      <c r="R22">
+        <v>7</v>
+      </c>
+      <c r="S22" t="str">
+        <f>VLOOKUP(R22,familias,2,FALSE)</f>
+        <v>parada2</v>
+      </c>
+      <c r="T22" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1275,8 +1705,22 @@
       <c r="O23" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="Q23" t="s">
+        <v>44</v>
+      </c>
+      <c r="R23">
+        <v>7</v>
+      </c>
+      <c r="S23" t="str">
+        <f>VLOOKUP(R23,familias,2,FALSE)</f>
+        <v>parada2</v>
+      </c>
+      <c r="T23" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1311,8 +1755,22 @@
       <c r="O24" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="Q24" t="s">
+        <v>45</v>
+      </c>
+      <c r="R24">
+        <v>8</v>
+      </c>
+      <c r="S24" t="str">
+        <f>VLOOKUP(R24,familias,2,FALSE)</f>
+        <v>paradaRH</v>
+      </c>
+      <c r="T24" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1347,8 +1805,22 @@
       <c r="O25" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="Q25" t="s">
+        <v>46</v>
+      </c>
+      <c r="R25">
+        <v>1</v>
+      </c>
+      <c r="S25" t="str">
+        <f>VLOOKUP(R25,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T25" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1383,8 +1855,22 @@
       <c r="O26" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="Q26" t="s">
+        <v>47</v>
+      </c>
+      <c r="R26">
+        <v>1</v>
+      </c>
+      <c r="S26" t="str">
+        <f>VLOOKUP(R26,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T26" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1401,7 +1887,7 @@
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="I27">
         <f t="shared" si="0"/>
@@ -1419,8 +1905,22 @@
       <c r="O27" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="Q27" t="s">
+        <v>48</v>
+      </c>
+      <c r="R27">
+        <v>1</v>
+      </c>
+      <c r="S27" t="str">
+        <f>VLOOKUP(R27,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T27" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
       <c r="A28">
         <v>0</v>
       </c>
@@ -1455,8 +1955,22 @@
       <c r="O28" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="Q28" t="s">
+        <v>49</v>
+      </c>
+      <c r="R28">
+        <v>1</v>
+      </c>
+      <c r="S28" t="str">
+        <f>VLOOKUP(R28,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T28" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20">
       <c r="A29">
         <v>0.66666999999999998</v>
       </c>
@@ -1491,8 +2005,22 @@
       <c r="O29" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="Q29" t="s">
+        <v>50</v>
+      </c>
+      <c r="R29">
+        <v>1</v>
+      </c>
+      <c r="S29" t="str">
+        <f>VLOOKUP(R29,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T29" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1527,8 +2055,22 @@
       <c r="O30" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="Q30" t="s">
+        <v>51</v>
+      </c>
+      <c r="R30">
+        <v>1</v>
+      </c>
+      <c r="S30" t="str">
+        <f>VLOOKUP(R30,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T30" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1563,8 +2105,22 @@
       <c r="O31" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="32" spans="1:15">
+      <c r="Q31" t="s">
+        <v>52</v>
+      </c>
+      <c r="R31">
+        <v>1</v>
+      </c>
+      <c r="S31" t="str">
+        <f>VLOOKUP(R31,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T31" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1599,8 +2155,22 @@
       <c r="O32" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="36" spans="7:15">
+      <c r="Q32" t="s">
+        <v>53</v>
+      </c>
+      <c r="R32">
+        <v>1</v>
+      </c>
+      <c r="S32" t="str">
+        <f>VLOOKUP(R32,familias,2,FALSE)</f>
+        <v>normal2</v>
+      </c>
+      <c r="T32" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="7:21">
       <c r="G36" t="s">
         <v>14</v>
       </c>
@@ -1608,7 +2178,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="7:15">
+    <row r="37" spans="7:21">
       <c r="G37" s="1" t="s">
         <v>5</v>
       </c>
@@ -1624,7 +2194,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="7:15">
+    <row r="38" spans="7:21">
       <c r="G38" t="s">
         <v>8</v>
       </c>
@@ -1639,14 +2209,20 @@
         <f>COUNTIF($O$2:$O$32,M38)</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="39" spans="7:15">
+      <c r="T38">
+        <v>0</v>
+      </c>
+      <c r="U38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="7:21">
       <c r="G39" t="s">
         <v>11</v>
       </c>
       <c r="I39">
-        <f t="shared" ref="I39:I43" si="1">COUNTIF($G$2:$G$32,G39)</f>
-        <v>6</v>
+        <f t="shared" ref="I39:I43" si="2">COUNTIF($G$2:$G$32,G39)</f>
+        <v>0</v>
       </c>
       <c r="M39" t="s">
         <v>21</v>
@@ -1655,56 +2231,140 @@
         <f>COUNTIF($O$2:$O$32,M39)</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="7:15">
+      <c r="T39">
+        <v>1</v>
+      </c>
+      <c r="U39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="7:21">
       <c r="G40" t="s">
         <v>7</v>
       </c>
       <c r="I40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="7:15">
+      <c r="T40">
+        <v>2</v>
+      </c>
+      <c r="U40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="7:21">
       <c r="G41" t="s">
         <v>9</v>
       </c>
       <c r="I41">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="7:15">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="T41">
+        <v>3</v>
+      </c>
+      <c r="U41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="7:21">
       <c r="G42" t="s">
         <v>10</v>
       </c>
       <c r="I42">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="7:15">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="T42">
+        <v>4</v>
+      </c>
+      <c r="U42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="7:21">
       <c r="G43" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
-    </row>
-    <row r="44" spans="7:15">
+      <c r="T43">
+        <v>5</v>
+      </c>
+      <c r="U43" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="7:21">
       <c r="I44" s="3">
         <f>SUM(I38:I43)</f>
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="M44" s="3"/>
       <c r="O44" s="3">
         <f>SUM(O38:O43)</f>
         <v>31</v>
+      </c>
+      <c r="T44">
+        <v>6</v>
+      </c>
+      <c r="U44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="7:21">
+      <c r="T45">
+        <v>7</v>
+      </c>
+      <c r="U45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="7:21">
+      <c r="T46">
+        <v>8</v>
+      </c>
+      <c r="U46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="7:21">
+      <c r="T47">
+        <v>9</v>
+      </c>
+      <c r="U47" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="7:21">
+      <c r="T48">
+        <v>10</v>
+      </c>
+      <c r="U48" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="20:21">
+      <c r="T49">
+        <v>11</v>
+      </c>
+      <c r="U49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="20:21">
+      <c r="T50">
+        <v>12</v>
+      </c>
+      <c r="U50" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fully functional counting procedure
</commit_message>
<xml_diff>
--- a/xls/calculo_disponibilidade.xlsx
+++ b/xls/calculo_disponibilidade.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="22980" windowHeight="9528" tabRatio="179" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="22980" windowHeight="9528" tabRatio="296" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan3" sheetId="3" r:id="rId2"/>
+    <sheet name="DR" sheetId="4" r:id="rId3"/>
+    <sheet name="RH" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="familias">Plan1!$X$38:$Y$51</definedName>
@@ -18,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="80">
   <si>
     <t>indice_ld</t>
   </si>
@@ -228,6 +230,36 @@
   </si>
   <si>
     <t>real</t>
+  </si>
+  <si>
+    <t>2 normais</t>
+  </si>
+  <si>
+    <t>6 cr/d</t>
+  </si>
+  <si>
+    <t>0 cr/d</t>
+  </si>
+  <si>
+    <t>12 cr/d</t>
+  </si>
+  <si>
+    <t>18 cr/dia</t>
+  </si>
+  <si>
+    <t>total dias</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>dias</t>
+  </si>
+  <si>
+    <t>count</t>
   </si>
 </sst>
 </file>
@@ -288,6 +320,643 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pt-BR"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>histograma dos dias operando DR</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>histograma</c:v>
+          </c:tx>
+          <c:dLbls>
+            <c:showVal val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>DR!$H$6:$H$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DR!$I$6:$I$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="44791680"/>
+        <c:axId val="44793216"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="44791680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="44793216"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="44793216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="44791680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pt-BR"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Histograma dos</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> dias operando RH</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.607174103237096E-2"/>
+          <c:y val="0.15325240594925635"/>
+          <c:w val="0.88337270341207352"/>
+          <c:h val="0.73076771653543304"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>RH!$B$2:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>RH!$C$2:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="43966464"/>
+        <c:axId val="43968000"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="43966464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="43968000"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="43968000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="43966464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pt-BR"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Histograma dos</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> dias operando FP2</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.6071741032370933E-2"/>
+          <c:y val="0.1532524059492564"/>
+          <c:w val="0.88337270341207352"/>
+          <c:h val="0.73076771653543326"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>RH!$E$2:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>RH!$F$2:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="157575424"/>
+        <c:axId val="157577216"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="157575424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="157577216"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="157577216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="157575424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000014" footer="0.31496062000000014"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -577,8 +1246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:Y51"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="W24" sqref="W24"/>
+    <sheetView topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2:Y32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -593,10 +1262,10 @@
     <col min="18" max="18" width="1.6640625" customWidth="1"/>
     <col min="19" max="19" width="8.88671875" customWidth="1"/>
     <col min="20" max="20" width="1.6640625" customWidth="1"/>
-    <col min="24" max="24" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24">
+    <row r="1" spans="2:25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -651,8 +1320,11 @@
       <c r="X1" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="2:24">
+      <c r="Y1" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="2:25">
       <c r="B2">
         <v>1</v>
       </c>
@@ -711,8 +1383,12 @@
         <f>W2=S2</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:24">
+      <c r="Y2">
+        <f>IF(AND(L2="normal2",S2="normal1"),1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -771,8 +1447,12 @@
         <f t="shared" ref="X3:X32" si="3">W3=S3</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:24">
+      <c r="Y3">
+        <f t="shared" ref="Y3:Y32" si="4">IF(AND(L3="normal2",S3="normal1"),1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -831,8 +1511,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:24">
+      <c r="Y4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:25">
       <c r="B5">
         <v>1</v>
       </c>
@@ -891,8 +1575,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:24">
+      <c r="Y5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25">
       <c r="B6">
         <v>1</v>
       </c>
@@ -951,8 +1639,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:24">
+      <c r="Y6">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:25">
       <c r="B7">
         <v>1</v>
       </c>
@@ -1011,8 +1703,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:24">
+      <c r="Y7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:25">
       <c r="B8">
         <v>1</v>
       </c>
@@ -1071,8 +1767,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:24">
+      <c r="Y8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25">
       <c r="B9">
         <v>1</v>
       </c>
@@ -1131,8 +1831,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:24">
+      <c r="Y9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:25">
       <c r="B10">
         <v>1</v>
       </c>
@@ -1191,8 +1895,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="2:24">
+      <c r="Y10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25">
       <c r="B11">
         <v>1</v>
       </c>
@@ -1251,8 +1959,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="2:24">
+      <c r="Y11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:25">
       <c r="B12">
         <v>1</v>
       </c>
@@ -1311,8 +2023,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="2:24">
+      <c r="Y12">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:25">
       <c r="B13">
         <v>1</v>
       </c>
@@ -1371,8 +2087,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="2:24">
+      <c r="Y13">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:25">
       <c r="B14">
         <v>1</v>
       </c>
@@ -1431,8 +2151,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="2:24">
+      <c r="Y14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:25">
       <c r="B15">
         <v>1</v>
       </c>
@@ -1491,8 +2215,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:24">
+      <c r="Y15">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:25">
       <c r="B16">
         <v>1</v>
       </c>
@@ -1551,8 +2279,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="2:24">
+      <c r="Y16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:25">
       <c r="B17">
         <v>1</v>
       </c>
@@ -1611,8 +2343,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:24">
+      <c r="Y17">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:25">
       <c r="B18">
         <v>1</v>
       </c>
@@ -1671,8 +2407,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="2:24">
+      <c r="Y18">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:25">
       <c r="B19">
         <v>1</v>
       </c>
@@ -1731,8 +2471,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="2:24">
+      <c r="Y19">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:25">
       <c r="B20">
         <v>1</v>
       </c>
@@ -1791,8 +2535,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="2:24">
+      <c r="Y20">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:25">
       <c r="B21">
         <v>1</v>
       </c>
@@ -1851,8 +2599,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="2:24">
+      <c r="Y21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:25">
       <c r="B22">
         <v>0</v>
       </c>
@@ -1911,8 +2663,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="2:24">
+      <c r="Y22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:25">
       <c r="B23">
         <v>0.79166999999999998</v>
       </c>
@@ -1971,8 +2727,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="2:24">
+      <c r="Y23">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:25">
       <c r="B24">
         <v>1</v>
       </c>
@@ -2031,8 +2791,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="2:24">
+      <c r="Y24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:25">
       <c r="B25">
         <v>1</v>
       </c>
@@ -2091,8 +2855,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="2:24">
+      <c r="Y25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:25">
       <c r="B26">
         <v>1</v>
       </c>
@@ -2151,8 +2919,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="2:24">
+      <c r="Y26">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:25">
       <c r="B27">
         <v>1</v>
       </c>
@@ -2211,8 +2983,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="2:24">
+      <c r="Y27">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:25">
       <c r="B28">
         <v>1</v>
       </c>
@@ -2271,8 +3047,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="2:24">
+      <c r="Y28">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:25">
       <c r="B29">
         <v>1</v>
       </c>
@@ -2331,8 +3111,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="2:24">
+      <c r="Y29">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:25">
       <c r="B30">
         <v>1</v>
       </c>
@@ -2391,8 +3175,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="2:24">
+      <c r="Y30">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:25">
       <c r="B31">
         <v>1</v>
       </c>
@@ -2451,8 +3239,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="2:24">
+      <c r="Y31">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:25">
       <c r="B32">
         <v>1</v>
       </c>
@@ -2509,6 +3301,10 @@
       </c>
       <c r="X32" t="b">
         <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -2631,10 +3427,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F12"/>
+  <dimension ref="B2:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2643,90 +3439,90 @@
     <col min="5" max="5" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6">
-      <c r="B1" s="2" t="s">
+    <row r="2" spans="2:6">
+      <c r="B2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="2:6">
-      <c r="B2" t="s">
+    <row r="3" spans="2:6">
+      <c r="B3" t="s">
         <v>60</v>
       </c>
-      <c r="F2">
+      <c r="F3">
         <f>COUNTIF(Plan1!$W$2:$W$32,"normal1")</f>
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:6">
-      <c r="B3" t="s">
+    <row r="4" spans="2:6">
+      <c r="B4" t="s">
         <v>61</v>
       </c>
-      <c r="F3">
+      <c r="F4">
         <f>COUNTIF(Plan1!$W$2:$W$32,"aciaria1")</f>
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="2" t="s">
+    <row r="7" spans="2:6">
+      <c r="B7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
-      <c r="B7" t="s">
+    <row r="8" spans="2:6">
+      <c r="B8" t="s">
         <v>63</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <f>COUNTIF(Plan1!$H$2:$H$32,"normal2")</f>
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
-      <c r="B8" t="s">
+    <row r="9" spans="2:6">
+      <c r="B9" t="s">
         <v>64</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <f>COUNTIF(Plan1!$H$2:$H$32,"aciaria2")</f>
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
-      <c r="B9" t="s">
+    <row r="10" spans="2:6">
+      <c r="B10" t="s">
         <v>65</v>
       </c>
-      <c r="F9">
+      <c r="F10">
         <f>COUNTIF(Plan1!$H$2:$H$32,"rh2")</f>
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
-      <c r="B10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10">
-        <f>COUNTIF(Plan1!$H$2:$H$32,"inspecao2")</f>
-        <v>1</v>
-      </c>
-    </row>
     <row r="11" spans="2:6">
       <c r="B11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F11">
-        <f>COUNTIF(Plan1!$H$2:$H$32,"mlc2")</f>
+        <f>COUNTIF(Plan1!$H$2:$H$32,"inspecao2")</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12">
+        <f>COUNTIF(Plan1!$H$2:$H$32,"mlc2")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" t="s">
         <v>68</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <f>COUNTIF(Plan1!$H$2:$H$32,"fp2")</f>
         <v>1</v>
       </c>
@@ -2734,4 +3530,1801 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I81"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>28</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <f>SUM(B2:D2)</f>
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2">
+        <f>MIN($E$2:$E$81)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E66" si="0">SUM(B3:D3)</f>
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3">
+        <f>MAX($E$2:$E$81)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>24</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>78</v>
+      </c>
+      <c r="I5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="H6">
+        <v>22</v>
+      </c>
+      <c r="I6">
+        <f>COUNTIF($E$2:$E$81,H6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>23</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="H7">
+        <v>23</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ref="I7:I15" si="1">COUNTIF($E$2:$E$81,H7)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="H8">
+        <v>24</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>21</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="H9">
+        <v>25</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="H10">
+        <v>26</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>18</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="H11">
+        <v>27</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>19</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="H12">
+        <v>28</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="H13">
+        <v>29</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <v>9</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="H14">
+        <v>30</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>17</v>
+      </c>
+      <c r="D15">
+        <v>9</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="H15">
+        <v>31</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>18</v>
+      </c>
+      <c r="D16">
+        <v>9</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>19</v>
+      </c>
+      <c r="D17">
+        <v>9</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>14</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>15</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <v>10</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>17</v>
+      </c>
+      <c r="D21">
+        <v>10</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>12</v>
+      </c>
+      <c r="D22">
+        <v>11</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>13</v>
+      </c>
+      <c r="D23">
+        <v>11</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>14</v>
+      </c>
+      <c r="D24">
+        <v>11</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>15</v>
+      </c>
+      <c r="D25">
+        <v>11</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>16</v>
+      </c>
+      <c r="D26">
+        <v>11</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>9</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>12</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <v>12</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+      <c r="D29">
+        <v>12</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>13</v>
+      </c>
+      <c r="D30">
+        <v>12</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>14</v>
+      </c>
+      <c r="D31">
+        <v>12</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>10</v>
+      </c>
+      <c r="C32">
+        <v>8</v>
+      </c>
+      <c r="D32">
+        <v>13</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>9</v>
+      </c>
+      <c r="D33">
+        <v>13</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="B34">
+        <v>6</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <v>13</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>11</v>
+      </c>
+      <c r="D35">
+        <v>13</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>12</v>
+      </c>
+      <c r="D36">
+        <v>13</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>13</v>
+      </c>
+      <c r="D37">
+        <v>13</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
+        <v>0</v>
+      </c>
+      <c r="B38">
+        <v>11</v>
+      </c>
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="D38">
+        <v>14</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>9</v>
+      </c>
+      <c r="C39">
+        <v>7</v>
+      </c>
+      <c r="D39">
+        <v>14</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="B40">
+        <v>7</v>
+      </c>
+      <c r="C40">
+        <v>8</v>
+      </c>
+      <c r="D40">
+        <v>14</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>3</v>
+      </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <v>9</v>
+      </c>
+      <c r="D41">
+        <v>14</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>4</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>10</v>
+      </c>
+      <c r="D42">
+        <v>14</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>5</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>11</v>
+      </c>
+      <c r="D43">
+        <v>14</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>0</v>
+      </c>
+      <c r="B44">
+        <v>12</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>15</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>10</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+      <c r="D45">
+        <v>15</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>2</v>
+      </c>
+      <c r="B46">
+        <v>8</v>
+      </c>
+      <c r="C46">
+        <v>6</v>
+      </c>
+      <c r="D46">
+        <v>15</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
+        <v>3</v>
+      </c>
+      <c r="B47">
+        <v>6</v>
+      </c>
+      <c r="C47">
+        <v>7</v>
+      </c>
+      <c r="D47">
+        <v>15</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48">
+        <v>4</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48">
+        <v>8</v>
+      </c>
+      <c r="D48">
+        <v>15</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>5</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49">
+        <v>9</v>
+      </c>
+      <c r="D49">
+        <v>15</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50">
+        <v>6</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>10</v>
+      </c>
+      <c r="D50">
+        <v>15</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51">
+        <v>0</v>
+      </c>
+      <c r="B51">
+        <v>13</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51">
+        <v>16</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>11</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52">
+        <v>16</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53">
+        <v>2</v>
+      </c>
+      <c r="B53">
+        <v>9</v>
+      </c>
+      <c r="C53">
+        <v>4</v>
+      </c>
+      <c r="D53">
+        <v>16</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54">
+        <v>3</v>
+      </c>
+      <c r="B54">
+        <v>7</v>
+      </c>
+      <c r="C54">
+        <v>5</v>
+      </c>
+      <c r="D54">
+        <v>16</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55">
+        <v>4</v>
+      </c>
+      <c r="B55">
+        <v>5</v>
+      </c>
+      <c r="C55">
+        <v>6</v>
+      </c>
+      <c r="D55">
+        <v>16</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56">
+        <v>5</v>
+      </c>
+      <c r="B56">
+        <v>3</v>
+      </c>
+      <c r="C56">
+        <v>7</v>
+      </c>
+      <c r="D56">
+        <v>16</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57">
+        <v>6</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>8</v>
+      </c>
+      <c r="D57">
+        <v>16</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58">
+        <v>0</v>
+      </c>
+      <c r="B58">
+        <v>14</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>17</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59">
+        <v>12</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>17</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60">
+        <v>2</v>
+      </c>
+      <c r="B60">
+        <v>10</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="D60">
+        <v>17</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61">
+        <v>3</v>
+      </c>
+      <c r="B61">
+        <v>8</v>
+      </c>
+      <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61">
+        <v>17</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62">
+        <v>4</v>
+      </c>
+      <c r="B62">
+        <v>6</v>
+      </c>
+      <c r="C62">
+        <v>4</v>
+      </c>
+      <c r="D62">
+        <v>17</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63">
+        <v>5</v>
+      </c>
+      <c r="B63">
+        <v>4</v>
+      </c>
+      <c r="C63">
+        <v>5</v>
+      </c>
+      <c r="D63">
+        <v>17</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64">
+        <v>6</v>
+      </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64">
+        <v>6</v>
+      </c>
+      <c r="D64">
+        <v>17</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65">
+        <v>7</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>7</v>
+      </c>
+      <c r="D65">
+        <v>17</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66">
+        <v>2</v>
+      </c>
+      <c r="B66">
+        <v>11</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>18</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67">
+        <v>3</v>
+      </c>
+      <c r="B67">
+        <v>9</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>18</v>
+      </c>
+      <c r="E67">
+        <f t="shared" ref="E67:E81" si="2">SUM(B67:D67)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68">
+        <v>4</v>
+      </c>
+      <c r="B68">
+        <v>7</v>
+      </c>
+      <c r="C68">
+        <v>2</v>
+      </c>
+      <c r="D68">
+        <v>18</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69">
+        <v>5</v>
+      </c>
+      <c r="B69">
+        <v>5</v>
+      </c>
+      <c r="C69">
+        <v>3</v>
+      </c>
+      <c r="D69">
+        <v>18</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70">
+        <v>6</v>
+      </c>
+      <c r="B70">
+        <v>3</v>
+      </c>
+      <c r="C70">
+        <v>4</v>
+      </c>
+      <c r="D70">
+        <v>18</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71">
+        <v>7</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>5</v>
+      </c>
+      <c r="D71">
+        <v>18</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72">
+        <v>4</v>
+      </c>
+      <c r="B72">
+        <v>8</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>19</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73">
+        <v>5</v>
+      </c>
+      <c r="B73">
+        <v>6</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>19</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74">
+        <v>6</v>
+      </c>
+      <c r="B74">
+        <v>4</v>
+      </c>
+      <c r="C74">
+        <v>2</v>
+      </c>
+      <c r="D74">
+        <v>19</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75">
+        <v>7</v>
+      </c>
+      <c r="B75">
+        <v>2</v>
+      </c>
+      <c r="C75">
+        <v>3</v>
+      </c>
+      <c r="D75">
+        <v>19</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76">
+        <v>8</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>4</v>
+      </c>
+      <c r="D76">
+        <v>19</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77">
+        <v>6</v>
+      </c>
+      <c r="B77">
+        <v>5</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>20</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78">
+        <v>7</v>
+      </c>
+      <c r="B78">
+        <v>3</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <v>20</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79">
+        <v>8</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79">
+        <v>2</v>
+      </c>
+      <c r="D79">
+        <v>20</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80">
+        <v>8</v>
+      </c>
+      <c r="B80">
+        <v>2</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>21</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81">
+        <v>9</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <v>21</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:F19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="2:6">
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6">
+      <c r="B2">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>22</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>23</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>24</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>31</v>
+      </c>
+      <c r="E5">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>46</v>
+      </c>
+      <c r="E6">
+        <v>26</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7">
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>62</v>
+      </c>
+      <c r="E7">
+        <v>27</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>76</v>
+      </c>
+      <c r="E8">
+        <v>28</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>87</v>
+      </c>
+      <c r="E9">
+        <v>29</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10">
+        <v>22</v>
+      </c>
+      <c r="C10">
+        <v>96</v>
+      </c>
+      <c r="E10">
+        <v>30</v>
+      </c>
+      <c r="F10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11">
+        <v>23</v>
+      </c>
+      <c r="C11">
+        <v>103</v>
+      </c>
+      <c r="E11">
+        <v>31</v>
+      </c>
+      <c r="F11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14">
+        <v>26</v>
+      </c>
+      <c r="C14">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15">
+        <v>27</v>
+      </c>
+      <c r="C15">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16">
+        <v>28</v>
+      </c>
+      <c r="C16">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17">
+        <v>29</v>
+      </c>
+      <c r="C17">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18">
+        <v>30</v>
+      </c>
+      <c r="C18">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19">
+        <v>31</v>
+      </c>
+      <c r="C19">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>